<commit_message>
Massa de dados para o teste
</commit_message>
<xml_diff>
--- a/MassaDeDados.xlsx
+++ b/MassaDeDados.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\PROJETO_BDD_HUB - ANGRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Documents\web_motors_project\BDD_TESTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82EFD52-DAC0-404C-A94E-9B6F287C7246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82BD26A-C5D1-4157-BDA5-93E0CA86E71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{99C58611-E9A4-44C3-A823-EF414D5520B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{99C58611-E9A4-44C3-A823-EF414D5520B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Teste" sheetId="1" r:id="rId1"/>
+    <sheet name="TesteComSucesso" sheetId="1" r:id="rId1"/>
+    <sheet name="TesteComFalha" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,25 +34,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
-    <t>MODELO</t>
+    <t>EMAIL</t>
   </si>
   <si>
-    <t>MARCA</t>
+    <t>SENHA</t>
   </si>
   <si>
-    <t>City</t>
+    <t>teste1@teste.com</t>
   </si>
   <si>
-    <t>Honda</t>
+    <t>teste123</t>
+  </si>
+  <si>
+    <t>teste1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +77,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -109,15 +127,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,27 +457,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0648F2-4C7C-4B3F-8F6B-7521C3D06092}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -462,4 +489,41 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A635465E-FB0D-4D27-8D5D-A8D6FE83350B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>